<commit_message>
First level code and generated code for SoAd
</commit_message>
<xml_diff>
--- a/tools/exacfg/analysis/AUTOSAR_SWS_TcpIp.xlsx
+++ b/tools/exacfg/analysis/AUTOSAR_SWS_TcpIp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\labs\zephyr-lab\Car-OS.Zephyr\car-os\tools\exacfg\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B9FC91-4074-42C9-B102-DB2D354114EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B61044C-4FEF-474B-982B-FF1F46E14103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="316">
   <si>
     <t>TcpIp</t>
   </si>
@@ -1616,9 +1616,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1656,7 +1656,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1762,7 +1762,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1904,7 +1904,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1914,8 +1914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E163" sqref="E163"/>
+    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D180" sqref="D180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2345,6 +2345,9 @@
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>1</v>
+      </c>
       <c r="C38" t="s">
         <v>43</v>
       </c>
@@ -2480,7 +2483,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E49" t="s">
         <v>55</v>
       </c>
@@ -2488,7 +2491,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F50" t="s">
         <v>56</v>
       </c>
@@ -2502,7 +2505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F51" t="s">
         <v>57</v>
       </c>
@@ -2516,7 +2519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E52" t="s">
         <v>58</v>
       </c>
@@ -2524,7 +2527,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F53" t="s">
         <v>59</v>
       </c>
@@ -2538,7 +2541,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F54" t="s">
         <v>60</v>
       </c>
@@ -2552,7 +2555,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F55" t="s">
         <v>61</v>
       </c>
@@ -2566,7 +2569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F56" t="s">
         <v>62</v>
       </c>
@@ -2574,7 +2577,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
       <c r="G57" t="s">
         <v>63</v>
       </c>
@@ -2588,7 +2591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
       <c r="G58" t="s">
         <v>64</v>
       </c>
@@ -2602,7 +2605,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <v>2</v>
+      </c>
       <c r="C59" t="s">
         <v>65</v>
       </c>
@@ -2610,7 +2616,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D60" t="s">
         <v>66</v>
       </c>
@@ -2624,7 +2630,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D61" t="s">
         <v>68</v>
       </c>
@@ -2638,7 +2644,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D62" t="s">
         <v>69</v>
       </c>
@@ -2652,7 +2658,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D63" t="s">
         <v>70</v>
       </c>
@@ -2660,7 +2666,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E64" t="s">
         <v>71</v>
       </c>
@@ -2674,7 +2680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E65" t="s">
         <v>72</v>
       </c>
@@ -2688,7 +2694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E66" t="s">
         <v>73</v>
       </c>
@@ -2702,7 +2708,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <v>3</v>
+      </c>
       <c r="C67" t="s">
         <v>74</v>
       </c>
@@ -2710,7 +2719,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D68" t="s">
         <v>75</v>
       </c>
@@ -2724,7 +2733,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>4</v>
+      </c>
       <c r="C69" t="s">
         <v>77</v>
       </c>
@@ -2732,7 +2744,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="70" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D70" t="s">
         <v>78</v>
       </c>
@@ -2740,7 +2752,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E71" t="s">
         <v>79</v>
       </c>
@@ -2748,7 +2760,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F72" t="s">
         <v>80</v>
       </c>
@@ -2762,7 +2774,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F73" t="s">
         <v>81</v>
       </c>
@@ -2776,7 +2788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F74" t="s">
         <v>82</v>
       </c>
@@ -2790,7 +2802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F75" t="s">
         <v>83</v>
       </c>
@@ -2804,7 +2816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F76" t="s">
         <v>84</v>
       </c>
@@ -2818,7 +2830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F77" t="s">
         <v>85</v>
       </c>
@@ -2832,7 +2844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E78" t="s">
         <v>86</v>
       </c>
@@ -2840,7 +2852,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F79" t="s">
         <v>87</v>
       </c>
@@ -2854,7 +2866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E80" t="s">
         <v>88</v>
       </c>
@@ -3674,7 +3686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:12" x14ac:dyDescent="0.3">
       <c r="I145" t="s">
         <v>154</v>
       </c>
@@ -3688,7 +3700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F146" t="s">
         <v>155</v>
       </c>
@@ -3696,7 +3708,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="147" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F147" t="s">
         <v>156</v>
       </c>
@@ -3710,7 +3722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F148" t="s">
         <v>157</v>
       </c>
@@ -3724,7 +3736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F149" t="s">
         <v>158</v>
       </c>
@@ -3738,7 +3750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F150" t="s">
         <v>159</v>
       </c>
@@ -3752,7 +3764,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B151">
+        <v>5</v>
+      </c>
       <c r="C151" s="1" t="s">
         <v>160</v>
       </c>
@@ -3764,7 +3779,7 @@
       <c r="G151" s="1"/>
       <c r="H151" s="1"/>
     </row>
-    <row r="152" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C152" s="1"/>
       <c r="D152" s="1" t="s">
         <v>161</v>
@@ -3780,7 +3795,7 @@
       </c>
       <c r="H152" s="1"/>
     </row>
-    <row r="153" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C153" s="1"/>
       <c r="D153" s="1" t="s">
         <v>163</v>
@@ -3796,7 +3811,7 @@
       </c>
       <c r="H153" s="1"/>
     </row>
-    <row r="154" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C154" s="1"/>
       <c r="D154" s="1" t="s">
         <v>164</v>
@@ -3812,7 +3827,7 @@
       </c>
       <c r="H154" s="1"/>
     </row>
-    <row r="155" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C155" s="1"/>
       <c r="D155" s="1" t="s">
         <v>165</v>
@@ -3828,7 +3843,7 @@
       </c>
       <c r="H155" s="1"/>
     </row>
-    <row r="156" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C156" s="1"/>
       <c r="D156" s="1" t="s">
         <v>166</v>
@@ -3844,7 +3859,7 @@
       </c>
       <c r="H156" s="1"/>
     </row>
-    <row r="157" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C157" s="1"/>
       <c r="D157" s="1" t="s">
         <v>168</v>
@@ -3856,7 +3871,7 @@
       <c r="G157" s="1"/>
       <c r="H157" s="1"/>
     </row>
-    <row r="158" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C158" s="1"/>
       <c r="D158" s="1"/>
       <c r="E158" s="1" t="s">
@@ -3872,7 +3887,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="159" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
       <c r="E159" s="1" t="s">
@@ -3888,7 +3903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
       <c r="E160" s="1" t="s">
@@ -3904,7 +3919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
       <c r="E161" s="1" t="s">
@@ -3920,7 +3935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C162" s="1"/>
       <c r="D162" s="1" t="s">
         <v>173</v>
@@ -3932,7 +3947,7 @@
       <c r="G162" s="1"/>
       <c r="H162" s="1"/>
     </row>
-    <row r="163" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
       <c r="E163" s="1" t="s">
@@ -3948,7 +3963,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="164" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
       <c r="E164" s="1" t="s">
@@ -3964,7 +3979,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="165" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C165" s="1"/>
       <c r="D165" s="1"/>
       <c r="E165" s="1" t="s">
@@ -3980,7 +3995,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B166">
+        <v>6</v>
+      </c>
       <c r="C166" t="s">
         <v>177</v>
       </c>
@@ -3988,7 +4006,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="167" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D167" t="s">
         <v>178</v>
       </c>
@@ -4002,7 +4020,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B168">
+        <v>7</v>
+      </c>
       <c r="C168" t="s">
         <v>179</v>
       </c>
@@ -4010,7 +4031,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="169" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D169" t="s">
         <v>180</v>
       </c>
@@ -4018,7 +4039,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="170" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D170" t="s">
         <v>181</v>
       </c>
@@ -4032,7 +4053,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B171">
+        <v>8</v>
+      </c>
       <c r="C171" t="s">
         <v>182</v>
       </c>
@@ -4040,155 +4064,173 @@
         <v>42</v>
       </c>
     </row>
-    <row r="172" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D172" t="s">
+    <row r="172" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D172" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E172" t="s">
+      <c r="E172" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="173" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E173" t="s">
+      <c r="F172" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G172" s="1"/>
+      <c r="H172" s="1"/>
+    </row>
+    <row r="173" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D173" s="1"/>
+      <c r="E173" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="F173" t="s">
+      <c r="F173" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G173" t="s">
+      <c r="G173" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="H173" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="174" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E174" t="s">
+      <c r="H173" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="174" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D174" s="1"/>
+      <c r="E174" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="F174" t="s">
+      <c r="F174" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G174" t="s">
+      <c r="G174" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H174" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="175" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E175" t="s">
+      <c r="H174" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="175" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D175" s="1"/>
+      <c r="E175" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F175" t="s">
+      <c r="F175" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G175" t="s">
+      <c r="G175" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H175">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="176" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E176" t="s">
+      <c r="H175" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D176" s="1"/>
+      <c r="E176" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="F176" t="s">
+      <c r="F176" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G176" t="s">
+      <c r="G176" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H176" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="177" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E177" t="s">
+      <c r="H176" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="177" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D177" s="1"/>
+      <c r="E177" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="F177" t="s">
+      <c r="F177" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G177" t="s">
+      <c r="G177" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="H177" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="178" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E178" t="s">
+      <c r="H177" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="178" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D178" s="1"/>
+      <c r="E178" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="F178" t="s">
+      <c r="F178" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G178" t="s">
+      <c r="G178" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="H178" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="179" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E179" t="s">
+      <c r="H178" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="179" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D179" s="1"/>
+      <c r="E179" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="F179" t="s">
+      <c r="F179" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G179" t="s">
+      <c r="G179" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="H179" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="180" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E180" t="s">
+      <c r="H179" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="180" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D180" s="1"/>
+      <c r="E180" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="F180" t="s">
+      <c r="F180" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G180" t="s">
+      <c r="G180" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="H180" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="181" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E181" t="s">
+      <c r="H180" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="181" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D181" s="1"/>
+      <c r="E181" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="F181" t="s">
+      <c r="F181" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G181" t="s">
+      <c r="G181" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="H181" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="182" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E182" t="s">
+      <c r="H181" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="182" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D182" s="1"/>
+      <c r="E182" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="F182" t="s">
+      <c r="F182" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G182" t="s">
+      <c r="G182" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="H182">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="183" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="H182" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B183">
+        <v>9</v>
+      </c>
       <c r="C183" t="s">
         <v>195</v>
       </c>
@@ -4196,7 +4238,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="184" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D184" t="s">
         <v>196</v>
       </c>
@@ -4210,7 +4252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D185" t="s">
         <v>197</v>
       </c>
@@ -4224,7 +4266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D186" t="s">
         <v>198</v>
       </c>
@@ -4238,7 +4280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D187" t="s">
         <v>199</v>
       </c>
@@ -4252,7 +4294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D188" t="s">
         <v>200</v>
       </c>
@@ -4266,7 +4308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D189" t="s">
         <v>201</v>
       </c>
@@ -4280,7 +4322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D190" t="s">
         <v>202</v>
       </c>
@@ -4294,7 +4336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D191" t="s">
         <v>203</v>
       </c>
@@ -4308,7 +4350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D192" t="s">
         <v>204</v>
       </c>
@@ -4322,7 +4364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D193" t="s">
         <v>205</v>
       </c>
@@ -4336,7 +4378,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="194" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D194" t="s">
         <v>206</v>
       </c>
@@ -4350,7 +4392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D195" t="s">
         <v>207</v>
       </c>
@@ -4364,7 +4406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D196" t="s">
         <v>208</v>
       </c>
@@ -4378,7 +4420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D197" t="s">
         <v>209</v>
       </c>
@@ -4392,7 +4434,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="198" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D198" t="s">
         <v>210</v>
       </c>
@@ -4406,7 +4448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D199" t="s">
         <v>211</v>
       </c>
@@ -4420,7 +4462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D200" t="s">
         <v>212</v>
       </c>
@@ -4434,7 +4476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D201" t="s">
         <v>213</v>
       </c>
@@ -4448,7 +4490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D202" t="s">
         <v>214</v>
       </c>
@@ -4456,7 +4498,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="203" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E203" t="s">
         <v>215</v>
       </c>
@@ -4470,7 +4512,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="204" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E204" t="s">
         <v>217</v>
       </c>
@@ -4484,7 +4526,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B205">
+        <v>10</v>
+      </c>
       <c r="C205" t="s">
         <v>218</v>
       </c>
@@ -4492,7 +4537,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="206" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D206" t="s">
         <v>219</v>
       </c>
@@ -4506,7 +4551,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B207">
+        <v>11</v>
+      </c>
       <c r="C207" t="s">
         <v>220</v>
       </c>
@@ -4514,7 +4562,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="208" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D208" t="s">
         <v>221</v>
       </c>
@@ -5376,7 +5424,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="273" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="273" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F273" t="s">
         <v>286</v>
       </c>
@@ -5390,7 +5438,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="274" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="274" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F274" t="s">
         <v>287</v>
       </c>
@@ -5404,7 +5452,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="275" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="275" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B275">
+        <v>12</v>
+      </c>
       <c r="C275" t="s">
         <v>288</v>
       </c>
@@ -5412,7 +5463,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="276" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="276" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D276" t="s">
         <v>289</v>
       </c>
@@ -5426,7 +5477,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="277" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="277" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D277" t="s">
         <v>290</v>
       </c>
@@ -5440,7 +5491,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="278" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="278" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D278" t="s">
         <v>291</v>
       </c>
@@ -5454,7 +5505,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="279" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="279" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D279" t="s">
         <v>292</v>
       </c>
@@ -5468,7 +5519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="280" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D280" t="s">
         <v>293</v>
       </c>
@@ -5476,7 +5527,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="281" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="281" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E281" t="s">
         <v>294</v>
       </c>
@@ -5490,7 +5541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="282" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E282" t="s">
         <v>295</v>
       </c>
@@ -5498,7 +5549,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="283" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="283" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E283" t="s">
         <v>296</v>
       </c>
@@ -5512,7 +5563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="284" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E284" t="s">
         <v>297</v>
       </c>
@@ -5526,7 +5577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="285" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D285" t="s">
         <v>298</v>
       </c>
@@ -5534,7 +5585,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="286" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="286" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E286" t="s">
         <v>299</v>
       </c>
@@ -5548,7 +5599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="287" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E287" t="s">
         <v>300</v>
       </c>
@@ -5556,7 +5607,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="288" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="288" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F288" t="s">
         <v>301</v>
       </c>
@@ -5771,10 +5822,15 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>